<commit_message>
finalized results and cleaned up outputs
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -497,16 +497,16 @@
         <v>10868846.75440167</v>
       </c>
       <c r="F2" t="n">
-        <v>22700277.53866357</v>
+        <v>22700277.5386635</v>
       </c>
       <c r="G2" t="n">
-        <v>8560876.209018489</v>
+        <v>8560876.20901845</v>
       </c>
       <c r="H2" t="n">
-        <v>6.118619293389627</v>
+        <v>6.118619293389694</v>
       </c>
       <c r="I2" t="n">
-        <v>2307.970545383173</v>
+        <v>2307.970545383213</v>
       </c>
     </row>
     <row r="3">
@@ -526,16 +526,16 @@
         <v>49207694.01521884</v>
       </c>
       <c r="F3" t="n">
-        <v>102773570.4964267</v>
+        <v>102773570.4964264</v>
       </c>
       <c r="G3" t="n">
-        <v>38758637.06134862</v>
+        <v>38758637.06134845</v>
       </c>
       <c r="H3" t="n">
-        <v>27.70130727308697</v>
+        <v>27.70130727308727</v>
       </c>
       <c r="I3" t="n">
-        <v>10449.05695387022</v>
+        <v>10449.0569538704</v>
       </c>
     </row>
     <row r="4">
@@ -555,16 +555,16 @@
         <v>109916258.2280364</v>
       </c>
       <c r="F4" t="n">
-        <v>229567525.0913672</v>
+        <v>229567525.0913665</v>
       </c>
       <c r="G4" t="n">
-        <v>86575997.57914513</v>
+        <v>86575997.57914473</v>
       </c>
       <c r="H4" t="n">
-        <v>61.8769458968865</v>
+        <v>61.87694589688716</v>
       </c>
       <c r="I4" t="n">
-        <v>23340.26064889125</v>
+        <v>23340.26064889166</v>
       </c>
     </row>
     <row r="5">
@@ -584,16 +584,16 @@
         <v>234782079.7516582</v>
       </c>
       <c r="F5" t="n">
-        <v>490358341.933172</v>
+        <v>490358341.9331707</v>
       </c>
       <c r="G5" t="n">
-        <v>184927126.0531702</v>
+        <v>184927126.0531694</v>
       </c>
       <c r="H5" t="n">
-        <v>132.1695724633061</v>
+        <v>132.1695724633075</v>
       </c>
       <c r="I5" t="n">
-        <v>49854.95369848797</v>
+        <v>49854.95369848885</v>
       </c>
     </row>
     <row r="6">
@@ -613,16 +613,16 @@
         <v>489000600.7089588</v>
       </c>
       <c r="F6" t="n">
-        <v>1021311085.732574</v>
+        <v>1021311085.732572</v>
       </c>
       <c r="G6" t="n">
-        <v>385163476.9381708</v>
+        <v>385163476.938169</v>
       </c>
       <c r="H6" t="n">
-        <v>275.2807340992346</v>
+        <v>275.2807340992375</v>
       </c>
       <c r="I6" t="n">
-        <v>103837.1237707879</v>
+        <v>103837.1237707898</v>
       </c>
     </row>
     <row r="7">
@@ -642,16 +642,16 @@
         <v>1003267448.21625</v>
       </c>
       <c r="F7" t="n">
-        <v>2095392498.272068</v>
+        <v>2095392498.272062</v>
       </c>
       <c r="G7" t="n">
-        <v>790228042.6659602</v>
+        <v>790228042.6659565</v>
       </c>
       <c r="H7" t="n">
-        <v>564.7849422200164</v>
+        <v>564.7849422200225</v>
       </c>
       <c r="I7" t="n">
-        <v>213039.4055502897</v>
+        <v>213039.4055502934</v>
       </c>
     </row>
     <row r="8">
@@ -671,16 +671,16 @@
         <v>2039385426.871216</v>
       </c>
       <c r="F8" t="n">
-        <v>4259395571.523443</v>
+        <v>4259395571.52343</v>
       </c>
       <c r="G8" t="n">
-        <v>1606330951.458266</v>
+        <v>1606330951.458258</v>
       </c>
       <c r="H8" t="n">
-        <v>1148.062942826406</v>
+        <v>1148.062942826419</v>
       </c>
       <c r="I8" t="n">
-        <v>433054.4754129503</v>
+        <v>433054.4754129578</v>
       </c>
     </row>
     <row r="9">
@@ -700,16 +700,16 @@
         <v>4121471153.61997</v>
       </c>
       <c r="F9" t="n">
-        <v>8607973787.180944</v>
+        <v>8607973787.180918</v>
       </c>
       <c r="G9" t="n">
-        <v>3246295041.663496</v>
+        <v>3246295041.663481</v>
       </c>
       <c r="H9" t="n">
-        <v>2320.163673608893</v>
+        <v>2320.163673608918</v>
       </c>
       <c r="I9" t="n">
-        <v>875176.1119564734</v>
+        <v>875176.1119564887</v>
       </c>
     </row>
     <row r="10">
@@ -729,16 +729,16 @@
         <v>8298461908.505033</v>
       </c>
       <c r="F10" t="n">
-        <v>17331904010.83662</v>
+        <v>17331904010.83656</v>
       </c>
       <c r="G10" t="n">
-        <v>6536320328.534113</v>
+        <v>6536320328.534081</v>
       </c>
       <c r="H10" t="n">
-        <v>4671.581897366708</v>
+        <v>4671.581897366757</v>
       </c>
       <c r="I10" t="n">
-        <v>1762141.57997092</v>
+        <v>1762141.57997095</v>
       </c>
     </row>
     <row r="11">
@@ -758,16 +758,16 @@
         <v>16669087686.31869</v>
       </c>
       <c r="F11" t="n">
-        <v>34814527465.50486</v>
+        <v>34814527465.50475</v>
       </c>
       <c r="G11" t="n">
-        <v>13129480953.9333</v>
+        <v>13129480953.93324</v>
       </c>
       <c r="H11" t="n">
-        <v>9383.78784229717</v>
+        <v>9383.787842297268</v>
       </c>
       <c r="I11" t="n">
-        <v>3539606.732385383</v>
+        <v>3539606.732385445</v>
       </c>
     </row>
     <row r="12">
@@ -787,16 +787,16 @@
         <v>33431992665.66237</v>
       </c>
       <c r="F12" t="n">
-        <v>69824998915.71069</v>
+        <v>69824998915.71048</v>
       </c>
       <c r="G12" t="n">
-        <v>26332857577.51674</v>
+        <v>26332857577.5166</v>
       </c>
       <c r="H12" t="n">
-        <v>18820.38954247056</v>
+        <v>18820.38954247076</v>
       </c>
       <c r="I12" t="n">
-        <v>7099135.088145641</v>
+        <v>7099135.088145765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>